<commit_message>
Updated README, json and excel files
</commit_message>
<xml_diff>
--- a/app/laureates_data.xlsx
+++ b/app/laureates_data.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Nobel laureates in 2002 - 2024" sheetId="1" r:id="rId1"/>
+    <sheet name="Charts Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="1148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="1177">
   <si>
     <t>GIVEN NAME</t>
   </si>
@@ -49,10 +50,10 @@
     <t>https://en.wikipedia.org/wiki/Aaron_Ciechanover</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the discovery of ubiquitin-mediated protein degradation
 AWARD YEAR: 2004
-MOTIVATION: for the discovery of ubiquitin-mediated protein degradation</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Abdulrazak</t>
@@ -67,10 +68,10 @@
     <t>https://en.wikipedia.org/wiki/Abdulrazak_Gurnah</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for his uncompromising and compassionate penetration of the effects of colonialism and the fate of the refugee in the gulf between cultures and continents
 AWARD YEAR: 2021
-MOTIVATION: for his uncompromising and compassionate penetration of the effects of colonialism and the fate of the refugee in the gulf between cultures and continents</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Abhijit</t>
@@ -85,10 +86,10 @@
     <t>https://en.wikipedia.org/wiki/Abhijit_Banerjee</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for their experimental approach to alleviating global poverty
 AWARD YEAR: 2019
-MOTIVATION: for their experimental approach to alleviating global poverty</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Abiy</t>
@@ -103,10 +104,10 @@
     <t>https://en.wikipedia.org/wiki/Abiy_Ahmed</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for his efforts to achieve peace and international cooperation, and in particular for his decisive initiative to resolve the border conflict with neighbouring Eritrea
 AWARD YEAR: 2019
-MOTIVATION: for his efforts to achieve peace and international cooperation, and in particular for his decisive initiative to resolve the border conflict with neighbouring Eritrea</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Ada E.</t>
@@ -124,10 +125,10 @@
     <t>https://en.wikipedia.org/wiki/Ada_Yonath</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for studies of the structure and function of the ribosome
 AWARD YEAR: 2009
-MOTIVATION: for studies of the structure and function of the ribosome</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Adam G.</t>
@@ -142,10 +143,10 @@
     <t>https://en.wikipedia.org/wiki/Adam_Riess</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of the accelerating expansion of the Universe through observations of distant supernovae
 AWARD YEAR: 2011
-MOTIVATION: for the discovery of the accelerating expansion of the Universe through observations of distant supernovae</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Akira</t>
@@ -160,10 +161,10 @@
     <t>https://en.wikipedia.org/wiki/Akira_Suzuki_(chemist)</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for palladium-catalyzed cross couplings in organic synthesis
 AWARD YEAR: 2010
-MOTIVATION: for palladium-catalyzed cross couplings in organic synthesis</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Yoshino</t>
@@ -175,10 +176,10 @@
     <t>https://en.wikipedia.org/wiki/Akira_Yoshino</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the development of lithium-ion batteries
 AWARD YEAR: 2019
-MOTIVATION: for the development of lithium-ion batteries</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Al</t>
@@ -193,10 +194,10 @@
     <t>https://en.wikipedia.org/wiki/Al_Gore</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for their efforts to build up and disseminate greater knowledge about man-made climate change, and to lay the foundations for the measures that are needed to counteract such change
 AWARD YEAR: 2007
-MOTIVATION: for their efforts to build up and disseminate greater knowledge about man-made climate change, and to lay the foundations for the measures that are needed to counteract such change</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Alain</t>
@@ -211,10 +212,10 @@
     <t>https://en.wikipedia.org/wiki/Alain_Aspect</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for experiments with entangled photons, establishing the violation of Bell inequalities and  pioneering quantum information science
 AWARD YEAR: 2022
-MOTIVATION: for experiments with entangled photons, establishing the violation of Bell inequalities and  pioneering quantum information science</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Albert</t>
@@ -229,10 +230,10 @@
     <t>https://en.wikipedia.org/wiki/Albert_Fert</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of Giant Magnetoresistance
 AWARD YEAR: 2007
-MOTIVATION: for the discovery of Giant Magnetoresistance</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Aleksey</t>
@@ -247,10 +248,10 @@
     <t>https://en.wikipedia.org/wiki/Alexei_Ekimov</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the discovery and synthesis of quantum dots
 AWARD YEAR: 2023
-MOTIVATION: for the discovery and synthesis of quantum dots</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Ales</t>
@@ -265,10 +266,10 @@
     <t>https://en.wikipedia.org/wiki/Ales_Bialiatski</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: The Peace Prize laureates represent civil society in their home countries. They have for many years promoted the right to criticise power and protect the fundamental rights of citizens. They have made an outstanding effort to document war crimes, human right abuses and the abuse of power. Together they demonstrate the significance of civil society for peace and democracy.
 AWARD YEAR: 2022
-MOTIVATION: The Peace Prize laureates represent civil society in their home countries. They have for many years promoted the right to criticise power and protect the fundamental rights of citizens. They have made an outstanding effort to document war crimes, human right abuses and the abuse of power. Together they demonstrate the significance of civil society for peace and democracy.</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Alexei</t>
@@ -283,10 +284,10 @@
     <t>https://en.wikipedia.org/wiki/Alexei_Alexeyevich_Abrikosov</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for pioneering contributions to the theory of superconductors and superfluids
 AWARD YEAR: 2003
-MOTIVATION: for pioneering contributions to the theory of superconductors and superfluids</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Alice</t>
@@ -301,10 +302,10 @@
     <t>https://en.wikipedia.org/wiki/Alice_Munro</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: master of the contemporary short story
 AWARD YEAR: 2013
-MOTIVATION: master of the contemporary short story</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Alvin E.</t>
@@ -319,10 +320,10 @@
     <t>https://en.wikipedia.org/wiki/Alvin_E._Roth</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for the theory of stable allocations and the practice of market design
 AWARD YEAR: 2012
-MOTIVATION: for the theory of stable allocations and the practice of market design</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Andre</t>
@@ -337,10 +338,10 @@
     <t>https://en.wikipedia.org/wiki/Andre_Geim</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for groundbreaking experiments regarding the two-dimensional material graphene
 AWARD YEAR: 2010
-MOTIVATION: for groundbreaking experiments regarding the two-dimensional material graphene</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Andrea</t>
@@ -355,10 +356,10 @@
     <t>https://en.wikipedia.org/wiki/Andrea_M._Ghez</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of a supermassive compact object at the centre of our galaxy
 AWARD YEAR: 2020
-MOTIVATION: for the discovery of a supermassive compact object at the centre of our galaxy</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Andrew Z.</t>
@@ -373,10 +374,10 @@
     <t>https://en.wikipedia.org/wiki/Andrew_Fire</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discovery of RNA interference - gene silencing by double-stranded RNA
 AWARD YEAR: 2006
-MOTIVATION: for their discovery of RNA interference - gene silencing by double-stranded RNA</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Angus</t>
@@ -391,10 +392,10 @@
     <t>https://en.wikipedia.org/wiki/Angus_Deaton</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for his analysis of consumption, poverty, and welfare
 AWARD YEAR: 2015
-MOTIVATION: for his analysis of consumption, poverty, and welfare</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Anne</t>
@@ -409,10 +410,10 @@
     <t>https://en.wikipedia.org/wiki/Anne_L%27Huillier</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for experimental methods that generate attosecond pulses of light for the study of electron dynamics in matter
 AWARD YEAR: 2023
-MOTIVATION: for experimental methods that generate attosecond pulses of light for the study of electron dynamics in matter</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Annie</t>
@@ -427,10 +428,10 @@
     <t>https://en.wikipedia.org/wiki/Annie_Ernaux</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for the courage and clinical acuity with which she uncovers the roots, estrangements and  collective restraints of personal memory
 AWARD YEAR: 2022
-MOTIVATION: for the courage and clinical acuity with which she uncovers the roots, estrangements and  collective restraints of personal memory</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Anthony J.</t>
@@ -469,10 +470,10 @@
     <t>https://en.wikipedia.org/wiki/Ardem_Patapoutian</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries of receptors for temperature and touch
 AWARD YEAR: 2021
-MOTIVATION: for their discoveries of receptors for temperature and touch</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Arieh</t>
@@ -487,10 +488,10 @@
     <t>https://en.wikipedia.org/wiki/Arieh_Warshel</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the development of multiscale models for complex chemical systems
 AWARD YEAR: 2013
-MOTIVATION: for the development of multiscale models for complex chemical systems</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Arthur</t>
@@ -505,10 +506,10 @@
     <t>https://en.wikipedia.org/wiki/Arthur_Ashkin</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the optical tweezers and their application to biological systems
 AWARD YEAR: 2018
-MOTIVATION: for the optical tweezers and their application to biological systems</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Arthur B.</t>
@@ -523,10 +524,10 @@
     <t>https://en.wikipedia.org/wiki/Arthur_B._McDonald</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of neutrino oscillations, which shows that neutrinos have mass
 AWARD YEAR: 2015
-MOTIVATION: for the discovery of neutrino oscillations, which shows that neutrinos have mass</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Avram</t>
@@ -553,10 +554,10 @@
     <t>https://en.wikipedia.org/wiki/Aziz_Sancar</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for mechanistic studies of DNA repair
 AWARD YEAR: 2015
-MOTIVATION: for mechanistic studies of DNA repair</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Barack</t>
@@ -571,10 +572,10 @@
     <t>https://en.wikipedia.org/wiki/Barack_Obama</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for his extraordinary efforts to strengthen international diplomacy and cooperation between peoples
 AWARD YEAR: 2009
-MOTIVATION: for his extraordinary efforts to strengthen international diplomacy and cooperation between peoples</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Barry C.</t>
@@ -589,10 +590,10 @@
     <t>https://en.wikipedia.org/wiki/Barry_Barish</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for decisive contributions to the LIGO detector and the observation of gravitational waves
 AWARD YEAR: 2017
-MOTIVATION: for decisive contributions to the LIGO detector and the observation of gravitational waves</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Barry J.</t>
@@ -607,10 +608,10 @@
     <t>https://en.wikipedia.org/wiki/Barry_Marshall</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discovery of the bacterium &lt;i&gt;Helicobacter pylori&lt;/i&gt; and its role in gastritis and peptic ulcer disease
 AWARD YEAR: 2005
-MOTIVATION: for their discovery of the bacterium &lt;i&gt;Helicobacter pylori&lt;/i&gt; and its role in gastritis and peptic ulcer disease</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Ben</t>
@@ -625,10 +626,10 @@
     <t>https://en.wikipedia.org/wiki/Ben_Bernanke</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for research on banks and financial crises
 AWARD YEAR: 2022
-MOTIVATION: for research on banks and financial crises</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Bengt</t>
@@ -643,10 +644,10 @@
     <t>https://en.wikipedia.org/wiki/Bengt_Holmström</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for their contributions to contract theory
 AWARD YEAR: 2016
-MOTIVATION: for their contributions to contract theory</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Benjamin</t>
@@ -661,10 +662,10 @@
     <t>https://en.wikipedia.org/wiki/Benjamin_List</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the development of asymmetric organocatalysis
 AWARD YEAR: 2021
-MOTIVATION: for the development of asymmetric organocatalysis</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Bernard L.</t>
@@ -679,10 +680,10 @@
     <t>https://en.wikipedia.org/wiki/Ben_Feringa</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the design and synthesis of molecular machines
 AWARD YEAR: 2016
-MOTIVATION: for the design and synthesis of molecular machines</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Bob</t>
@@ -697,10 +698,10 @@
     <t>https://en.wikipedia.org/wiki/Bob_Dylan</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for having created new poetic expressions within the great American song tradition
 AWARD YEAR: 2016
-MOTIVATION: for having created new poetic expressions within the great American song tradition</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Brian</t>
@@ -715,10 +716,10 @@
     <t>https://en.wikipedia.org/wiki/Brian_Kobilka</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for studies of G-protein-coupled receptors
 AWARD YEAR: 2012
-MOTIVATION: for studies of G-protein-coupled receptors</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Brian P.</t>
@@ -745,10 +746,10 @@
     <t>https://en.wikipedia.org/wiki/Bruce_Beutler</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries concerning the activation of innate immunity
 AWARD YEAR: 2011
-MOTIVATION: for their discoveries concerning the activation of innate immunity</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Carol W.</t>
@@ -763,10 +764,10 @@
     <t>https://en.wikipedia.org/wiki/Carol_W._Greider</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for the discovery of how chromosomes are protected by telomeres and the enzyme telomerase
 AWARD YEAR: 2009
-MOTIVATION: for the discovery of how chromosomes are protected by telomeres and the enzyme telomerase</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Carolyn</t>
@@ -781,10 +782,10 @@
     <t>https://en.wikipedia.org/wiki/Carolyn_R._Bertozzi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the development of click chemistry and bioorthogonal chemistry
 AWARD YEAR: 2022
-MOTIVATION: for the development of click chemistry and bioorthogonal chemistry</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Charles K.</t>
@@ -799,10 +800,10 @@
     <t>https://en.wikipedia.org/wiki/Charles_K._Kao</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for groundbreaking achievements concerning the transmission of light in fibers for optical communication
 AWARD YEAR: 2009
-MOTIVATION: for groundbreaking achievements concerning the transmission of light in fibers for optical communication</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Charles</t>
@@ -817,10 +818,10 @@
     <t>https://en.wikipedia.org/wiki/Charles_M._Rice</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for the discovery of Hepatitis C virus
 AWARD YEAR: 2020
-MOTIVATION: for the discovery of Hepatitis C virus</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Christopher A.</t>
@@ -835,10 +836,10 @@
     <t>https://en.wikipedia.org/wiki/Christopher_A._Pissarides</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for their analysis of markets with search frictions
 AWARD YEAR: 2010
-MOTIVATION: for their analysis of markets with search frictions</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Sims</t>
@@ -850,10 +851,10 @@
     <t>https://en.wikipedia.org/wiki/Christopher_A._Sims</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for their empirical research on cause and effect in the macroeconomy
 AWARD YEAR: 2011
-MOTIVATION: for their empirical research on cause and effect in the macroeconomy</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Claudia</t>
@@ -868,10 +869,10 @@
     <t>https://en.wikipedia.org/wiki/Claudia_Goldin</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for having advanced our understanding of women’s labour market outcomes
 AWARD YEAR: 2023
-MOTIVATION: for having advanced our understanding of women’s labour market outcomes</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Clive W.J.</t>
@@ -886,10 +887,10 @@
     <t>https://en.wikipedia.org/wiki/Clive_Granger</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for methods of analyzing economic time series with common trends (cointegration)
 AWARD YEAR: 2003
-MOTIVATION: for methods of analyzing economic time series with common trends (cointegration)</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Craig C.</t>
@@ -928,10 +929,10 @@
     <t>https://en.wikipedia.org/wiki/Dan_Shechtman</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the discovery of quasicrystals
 AWARD YEAR: 2011
-MOTIVATION: for the discovery of quasicrystals</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Daniel</t>
@@ -946,10 +947,10 @@
     <t>https://en.wikipedia.org/wiki/Daniel_Kahneman</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for having integrated insights from psychological research into economic science, especially concerning human judgment and decision-making under uncertainty
 AWARD YEAR: 2002
-MOTIVATION: for having integrated insights from psychological research into economic science, especially concerning human judgment and decision-making under uncertainty</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>David</t>
@@ -964,10 +965,10 @@
     <t>https://en.wikipedia.org/wiki/David_Card</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for his empirical contributions to labour economics
 AWARD YEAR: 2021
-MOTIVATION: for his empirical contributions to labour economics</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>David J.</t>
@@ -982,10 +983,10 @@
     <t>https://en.wikipedia.org/wiki/David_Gross</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of asymptotic freedom in the theory of the strong interaction
 AWARD YEAR: 2004
-MOTIVATION: for the discovery of asymptotic freedom in the theory of the strong interaction</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Thouless</t>
@@ -997,10 +998,10 @@
     <t>https://en.wikipedia.org/wiki/David_J._Thouless</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for theoretical discoveries of topological phase transitions and topological phases of matter
 AWARD YEAR: 2016
-MOTIVATION: for theoretical discoveries of topological phase transitions and topological phases of matter</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Wineland</t>
@@ -1012,10 +1013,10 @@
     <t>https://en.wikipedia.org/wiki/David_J._Wineland</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for ground-breaking experimental methods that enable measuring and manipulation of individual quantum systems
 AWARD YEAR: 2012
-MOTIVATION: for ground-breaking experimental methods that enable measuring and manipulation of individual quantum systems</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Julius</t>
@@ -1048,10 +1049,10 @@
     <t>https://en.wikipedia.org/wiki/Denis_Mukwege</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for their efforts to end the use of sexual violence as a weapon of war and armed conflict
 AWARD YEAR: 2018
-MOTIVATION: for their efforts to end the use of sexual violence as a weapon of war and armed conflict</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Didier</t>
@@ -1066,10 +1067,10 @@
     <t>https://en.wikipedia.org/wiki/Didier_Queloz</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of an exoplanet orbiting a solar-type star
 AWARD YEAR: 2019
-MOTIVATION: for the discovery of an exoplanet orbiting a solar-type star</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Dmitry</t>
@@ -1084,10 +1085,10 @@
     <t>https://en.wikipedia.org/wiki/Dmitry_Muratov</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for their efforts to safeguard freedom of expression, which is a precondition for democracy and lasting peace
 AWARD YEAR: 2021
-MOTIVATION: for their efforts to safeguard freedom of expression, which is a precondition for democracy and lasting peace</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Donna</t>
@@ -1102,10 +1103,10 @@
     <t>https://en.wikipedia.org/wiki/Donna_Strickland</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for their method of generating high-intensity, ultra-short optical pulses
 AWARD YEAR: 2018
-MOTIVATION: for their method of generating high-intensity, ultra-short optical pulses</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Doris</t>
@@ -1120,10 +1121,10 @@
     <t>https://en.wikipedia.org/wiki/Doris_Lessing</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: that epicist of the female experience, who with scepticism, fire and visionary power has subjected a divided civilisation to scrutiny
 AWARD YEAR: 2007
-MOTIVATION: that epicist of the female experience, who with scepticism, fire and visionary power has subjected a divided civilisation to scrutiny</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Douglas</t>
@@ -1150,10 +1151,10 @@
     <t>https://en.wikipedia.org/wiki/Drew_Weissman</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries concerning nucleoside base modifications that enabled the development of effective mRNA vaccines against COVID-19
 AWARD YEAR: 2023
-MOTIVATION: for their discoveries concerning nucleoside base modifications that enabled the development of effective mRNA vaccines against COVID-19</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Edmund S.</t>
@@ -1168,10 +1169,10 @@
     <t>https://en.wikipedia.org/wiki/Edmund_Phelps</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for his analysis of intertemporal tradeoffs in macroeconomic policy
 AWARD YEAR: 2006
-MOTIVATION: for his analysis of intertemporal tradeoffs in macroeconomic policy</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Edvard I.</t>
@@ -1186,10 +1187,10 @@
     <t>https://en.wikipedia.org/wiki/Edvard_Moser</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries of cells that constitute a positioning system in the brain
 AWARD YEAR: 2014
-MOTIVATION: for their discoveries of cells that constitute a positioning system in the brain</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Edward C.</t>
@@ -1204,10 +1205,10 @@
     <t>https://en.wikipedia.org/wiki/Edward_C._Prescott</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for their contributions to dynamic macroeconomics: the time consistency of economic policy and the driving forces behind business cycles
 AWARD YEAR: 2004
-MOTIVATION: for their contributions to dynamic macroeconomics: the time consistency of economic policy and the driving forces behind business cycles</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Ei-ichi</t>
@@ -1234,10 +1235,10 @@
     <t>https://en.wikipedia.org/wiki/Elfriede_Jelinek</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for her musical flow of voices and counter-voices in novels and plays that with extraordinary linguistic zeal reveal the absurdity of society's clich&amp;eacute;s and their subjugating power
 AWARD YEAR: 2004
-MOTIVATION: for her musical flow of voices and counter-voices in novels and plays that with extraordinary linguistic zeal reveal the absurdity of society's clich&amp;eacute;s and their subjugating power</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Elinor</t>
@@ -1252,10 +1253,10 @@
     <t>https://en.wikipedia.org/wiki/Elinor_Ostrom</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for her analysis of economic governance, especially the commons
 AWARD YEAR: 2009
-MOTIVATION: for her analysis of economic governance, especially the commons</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Elizabeth H.</t>
@@ -1282,10 +1283,10 @@
     <t>https://en.wikipedia.org/wiki/Ellen_Johnson_Sirleaf</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for their non-violent struggle for the safety of women and for women's rights to full participation in peace-building work
 AWARD YEAR: 2011
-MOTIVATION: for their non-violent struggle for the safety of women and for women's rights to full participation in peace-building work</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Emmanuelle</t>
@@ -1300,10 +1301,10 @@
     <t>https://en.wikipedia.org/wiki/Emmanuelle_Charpentier</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the development of a method for genome editing
 AWARD YEAR: 2020
-MOTIVATION: for the development of a method for genome editing</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Eric</t>
@@ -1318,10 +1319,10 @@
     <t>https://en.wikipedia.org/wiki/Eric_Betzig</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the development of super-resolved fluorescence microscopy
 AWARD YEAR: 2014
-MOTIVATION: for the development of super-resolved fluorescence microscopy</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Eric S.</t>
@@ -1336,10 +1337,10 @@
     <t>https://en.wikipedia.org/wiki/Eric_Maskin</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for having laid the foundations of mechanism design theory
 AWARD YEAR: 2007
-MOTIVATION: for having laid the foundations of mechanism design theory</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Esther</t>
@@ -1366,10 +1367,10 @@
     <t>https://en.wikipedia.org/wiki/Eugene_Fama</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for their empirical analysis of asset prices
 AWARD YEAR: 2013
-MOTIVATION: for their empirical analysis of asset prices</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>F. Duncan M.</t>
@@ -1420,10 +1421,10 @@
     <t>https://en.wikipedia.org/wiki/Frances_Arnold</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the directed evolution of enzymes
 AWARD YEAR: 2018
-MOTIVATION: for the directed evolution of enzymes</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>François</t>
@@ -1438,10 +1439,10 @@
     <t>https://en.wikipedia.org/wiki/François_Englert</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the theoretical discovery of a mechanism that contributes to our understanding of the origin of mass of subatomic particles, and which recently was confirmed through the discovery of the predicted fundamental particle, by the ATLAS and CMS experiments at CERN's Large Hadron Collider
 AWARD YEAR: 2013
-MOTIVATION: for the theoretical discovery of a mechanism that contributes to our understanding of the origin of mass of subatomic particles, and which recently was confirmed through the discovery of the predicted fundamental particle, by the ATLAS and CMS experiments at CERN's Large Hadron Collider</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Françoise</t>
@@ -1456,10 +1457,10 @@
     <t>https://en.wikipedia.org/wiki/Françoise_Barré-Sinoussi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discovery of human immunodeficiency virus
 AWARD YEAR: 2008
-MOTIVATION: for their discovery of human immunodeficiency virus</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Frank</t>
@@ -1486,10 +1487,10 @@
     <t>https://en.wikipedia.org/wiki/George_E._Smith</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the invention of an imaging semiconductor circuit - the CCD sensor
 AWARD YEAR: 2009
-MOTIVATION: for the invention of an imaging semiconductor circuit - the CCD sensor</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>George F.</t>
@@ -1504,10 +1505,10 @@
     <t>https://en.wikipedia.org/wiki/George_Smoot</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for their discovery of the blackbody form and anisotropy of the cosmic microwave background radiation
 AWARD YEAR: 2006
-MOTIVATION: for their discovery of the blackbody form and anisotropy of the cosmic microwave background radiation</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>George P.</t>
@@ -1519,10 +1520,10 @@
     <t>https://en.wikipedia.org/wiki/George_Smith_(chemist)</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the phage display of peptides and antibodies
 AWARD YEAR: 2018
-MOTIVATION: for the phage display of peptides and antibodies</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Gérard</t>
@@ -1549,10 +1550,10 @@
     <t>https://en.wikipedia.org/wiki/Gerhard_Ertl</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for his studies of chemical processes on solid surfaces
 AWARD YEAR: 2007
-MOTIVATION: for his studies of chemical processes on solid surfaces</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Giorgio</t>
@@ -1567,10 +1568,10 @@
     <t>https://en.wikipedia.org/wiki/Giorgio_Parisi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of the interplay of disorder and fluctuations in physical systems from atomic to planetary scales
 AWARD YEAR: 2021
-MOTIVATION: for the discovery of the interplay of disorder and fluctuations in physical systems from atomic to planetary scales</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Gregg</t>
@@ -1585,10 +1586,10 @@
     <t>https://en.wikipedia.org/wiki/Gregg_L._Semenza</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries of how cells sense and adapt to oxygen availability
 AWARD YEAR: 2019
-MOTIVATION: for their discoveries of how cells sense and adapt to oxygen availability</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Guido</t>
@@ -1603,10 +1604,10 @@
     <t>https://en.wikipedia.org/wiki/Guido_Imbens</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for their methodological contributions to the analysis of causal relationships
 AWARD YEAR: 2021
-MOTIVATION: for their methodological contributions to the analysis of causal relationships</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>H. David</t>
@@ -1633,10 +1634,10 @@
     <t>https://en.wikipedia.org/wiki/H._Robert_Horvitz</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries concerning genetic regulation of organ development and programmed cell death'
 AWARD YEAR: 2002
-MOTIVATION: for their discoveries concerning genetic regulation of organ development and programmed cell death'</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Harald</t>
@@ -1651,10 +1652,10 @@
     <t>https://en.wikipedia.org/wiki/Harald_zur_Hausen</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for his discovery of human papilloma viruses causing cervical cancer
 AWARD YEAR: 2008
-MOTIVATION: for his discovery of human papilloma viruses causing cervical cancer</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Harold</t>
@@ -1669,10 +1670,10 @@
     <t>https://en.wikipedia.org/wiki/Harold_Pinter</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: who in his plays uncovers the precipice under everyday prattle and forces entry into oppression's closed rooms
 AWARD YEAR: 2005
-MOTIVATION: who in his plays uncovers the precipice under everyday prattle and forces entry into oppression's closed rooms</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Harvey</t>
@@ -1699,10 +1700,10 @@
     <t>https://en.wikipedia.org/wiki/Herta_Müller</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: who, with the concentration of poetry and the frankness of prose, depicts the landscape of the dispossessed
 AWARD YEAR: 2009
-MOTIVATION: who, with the concentration of poetry and the frankness of prose, depicts the landscape of the dispossessed</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Hiroshi</t>
@@ -1717,10 +1718,10 @@
     <t>https://en.wikipedia.org/wiki/Hiroshi_Amano</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the invention of efficient blue light-emitting diodes which has enabled bright and energy-saving white light sources
 AWARD YEAR: 2014
-MOTIVATION: for the invention of efficient blue light-emitting diodes which has enabled bright and energy-saving white light sources</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Imre</t>
@@ -1735,10 +1736,10 @@
     <t>https://en.wikipedia.org/wiki/Imre_Kertész</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for writing that upholds the fragile experience of the individual against the barbaric arbitrariness of history
 AWARD YEAR: 2002
-MOTIVATION: for writing that upholds the fragile experience of the individual against the barbaric arbitrariness of history</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Irwin</t>
@@ -1777,10 +1778,10 @@
     <t>https://en.wikipedia.org/wiki/J._M._Coetzee</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: who in innumerable guises portrays the surprising involvement of the outsider
 AWARD YEAR: 2003
-MOTIVATION: who in innumerable guises portrays the surprising involvement of the outsider</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>J. Michael</t>
@@ -1831,10 +1832,10 @@
     <t>https://en.wikipedia.org/wiki/Jacques_Dubochet</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for developing cryo-electron microscopy for the high-resolution structure determination of biomolecules in solution
 AWARD YEAR: 2017
-MOTIVATION: for developing cryo-electron microscopy for the high-resolution structure determination of biomolecules in solution</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>James E.</t>
@@ -1849,10 +1850,10 @@
     <t>https://en.wikipedia.org/wiki/James_Rothman</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries of machinery regulating vesicle traffic, a major transport system in our cells
 AWARD YEAR: 2013
-MOTIVATION: for their discoveries of machinery regulating vesicle traffic, a major transport system in our cells</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>James P.</t>
@@ -1867,10 +1868,10 @@
     <t>https://en.wikipedia.org/wiki/James_P._Allison</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discovery of cancer therapy by inhibition of negative immune regulation
 AWARD YEAR: 2018
-MOTIVATION: for their discovery of cancer therapy by inhibition of negative immune regulation</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>James</t>
@@ -1885,10 +1886,10 @@
     <t>https://en.wikipedia.org/wiki/Jim_Peebles</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for theoretical discoveries in physical cosmology
 AWARD YEAR: 2019
-MOTIVATION: for theoretical discoveries in physical cosmology</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Jean</t>
@@ -1903,10 +1904,10 @@
     <t>https://en.wikipedia.org/wiki/Jean_Tirole</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for his analysis of market power and regulation
 AWARD YEAR: 2014
-MOTIVATION: for his analysis of market power and regulation</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Jean-Marie Gustave</t>
@@ -1921,10 +1922,10 @@
     <t>https://en.wikipedia.org/wiki/J._M._G._Le_Clézio</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: author of new departures, poetic adventure and sensual ecstasy, explorer of a humanity beyond and below the reigning civilization
 AWARD YEAR: 2008
-MOTIVATION: author of new departures, poetic adventure and sensual ecstasy, explorer of a humanity beyond and below the reigning civilization</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Jean-Pierre</t>
@@ -1951,10 +1952,10 @@
     <t>https://en.wikipedia.org/wiki/Jeffrey_C._Hall</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries of molecular mechanisms controlling the circadian rhythm
 AWARD YEAR: 2017
-MOTIVATION: for their discoveries of molecular mechanisms controlling the circadian rhythm</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Jennifer A.</t>
@@ -1981,10 +1982,10 @@
     <t>https://en.wikipedia.org/wiki/Jimmy_Carter</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for his decades of untiring effort to find peaceful solutions to international conflicts, to advance democracy and human rights, and to promote economic and social development
 AWARD YEAR: 2002
-MOTIVATION: for his decades of untiring effort to find peaceful solutions to international conflicts, to advance democracy and human rights, and to promote economic and social development</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Joachim</t>
@@ -2008,10 +2009,10 @@
     <t>https://en.wikipedia.org/wiki/John_Fenn_(chemist)</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for their development of soft desorption ionisation methods for mass spectrometric analyses of biological macromolecules
 AWARD YEAR: 2002
-MOTIVATION: for their development of soft desorption ionisation methods for mass spectrometric analyses of biological macromolecules</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>John</t>
@@ -2071,10 +2072,10 @@
     <t>https://en.wikipedia.org/wiki/John_L._Hall</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for their contributions to the development of laser-based precision spectroscopy, including the optical frequency comb technique
 AWARD YEAR: 2005
-MOTIVATION: for their contributions to the development of laser-based precision spectroscopy, including the optical frequency comb technique</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>O'Keefe</t>
@@ -2098,10 +2099,10 @@
     <t>https://en.wikipedia.org/wiki/Jon_Fosse</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for his innovative plays and prose which give voice to the unsayable
 AWARD YEAR: 2023
-MOTIVATION: for his innovative plays and prose which give voice to the unsayable</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Joshua</t>
@@ -2128,10 +2129,10 @@
     <t>https://en.wikipedia.org/wiki/Juan_Manuel_Santos</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for his resolute efforts to bring the country's more than 50-year-long civil war to an end
 AWARD YEAR: 2016
-MOTIVATION: for his resolute efforts to bring the country's more than 50-year-long civil war to an end</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Jules A.</t>
@@ -2158,14 +2159,14 @@
     <t>https://en.wikipedia.org/wiki/Karl_Barry_Sharpless</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for his work on chirally catalysed oxidation reactions
 AWARD YEAR: 2001
-MOTIVATION: for his work on chirally catalysed oxidation reactions
 PRIZE STATUS: received
 CATEGORY: Chemistry
+MOTIVATION: for the development of click chemistry and bioorthogonal chemistry
 AWARD YEAR: 2022
-MOTIVATION: for the development of click chemistry and bioorthogonal chemistry</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Kailash</t>
@@ -2180,10 +2181,10 @@
     <t>https://en.wikipedia.org/wiki/Kailash_Satyarthi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for their struggle against the suppression of children and young people and for the right of all children to education
 AWARD YEAR: 2014
-MOTIVATION: for their struggle against the suppression of children and young people and for the right of all children to education</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Katalin</t>
@@ -2210,10 +2211,10 @@
     <t>https://en.wikipedia.org/wiki/Kazuo_Ishiguro</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: who, in novels of great emotional force, has uncovered the abyss beneath our illusory sense of connection with the world
 AWARD YEAR: 2017
-MOTIVATION: who, in novels of great emotional force, has uncovered the abyss beneath our illusory sense of connection with the world</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Kip S.</t>
@@ -2240,10 +2241,10 @@
     <t>https://en.wikipedia.org/wiki/Klaus_Hasselmann</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the physical modelling of Earth’s climate, quantifying variability and reliably predicting global warming
 AWARD YEAR: 2021
-MOTIVATION: for the physical modelling of Earth’s climate, quantifying variability and reliably predicting global warming</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Koichi</t>
@@ -2282,10 +2283,10 @@
     <t>https://en.wikipedia.org/wiki/Kurt_Wüthrich</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for his development of nuclear magnetic resonance spectroscopy for determining the three-dimensional structure of biological macromolecules in solution
 AWARD YEAR: 2002
-MOTIVATION: for his development of nuclear magnetic resonance spectroscopy for determining the three-dimensional structure of biological macromolecules in solution</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Lars Peter</t>
@@ -2336,10 +2337,10 @@
     <t>https://en.wikipedia.org/wiki/Linda_B._Buck</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries of odorant receptors and the organization of the olfactory system
 AWARD YEAR: 2004
-MOTIVATION: for their discoveries of odorant receptors and the organization of the olfactory system</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Xiaobo</t>
@@ -2354,10 +2355,10 @@
     <t>https://en.wikipedia.org/wiki/Liu_Xiaobo</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for his long and non-violent struggle for fundamental human rights in China
 AWARD YEAR: 2010
-MOTIVATION: for his long and non-violent struggle for fundamental human rights in China</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Lloyd S.</t>
@@ -2396,10 +2397,10 @@
     <t>https://en.wikipedia.org/wiki/Louise_Glück</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for her unmistakable poetic voice that with austere beauty makes individual existence universal
 AWARD YEAR: 2020
-MOTIVATION: for her unmistakable poetic voice that with austere beauty makes individual existence universal</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Luc</t>
@@ -2438,10 +2439,10 @@
     <t>https://en.wikipedia.org/wiki/Makoto_Kobayashi_(physicist)</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of the origin of the broken symmetry which predicts the existence of at least three families of quarks in nature
 AWARD YEAR: 2008
-MOTIVATION: for the discovery of the origin of the broken symmetry which predicts the existence of at least three families of quarks in nature</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Malala</t>
@@ -2480,10 +2481,10 @@
     <t>https://en.wikipedia.org/wiki/Mario_Capecchi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries of principles for introducing specific gene modifications in mice by the use of embryonic stem cells
 AWARD YEAR: 2007
-MOTIVATION: for their discoveries of principles for introducing specific gene modifications in mice by the use of embryonic stem cells</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Mario</t>
@@ -2498,10 +2499,10 @@
     <t>https://en.wikipedia.org/wiki/Mario_Vargas_Llosa</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for his cartography of structures of power and his trenchant images of the individual's resistance, revolt, and defeat
 AWARD YEAR: 2010
-MOTIVATION: for his cartography of structures of power and his trenchant images of the individual's resistance, revolt, and defeat</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Martin</t>
@@ -2516,10 +2517,10 @@
     <t>https://en.wikipedia.org/wiki/Martin_Chalfie</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the discovery and development of the green fluorescent protein, GFP
 AWARD YEAR: 2008
-MOTIVATION: for the discovery and development of the green fluorescent protein, GFP</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Karplus</t>
@@ -2543,10 +2544,10 @@
     <t>https://en.wikipedia.org/wiki/Martti_Ahtisaari</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for his important efforts, on several continents and over more than three decades, to resolve international conflicts
 AWARD YEAR: 2008
-MOTIVATION: for his important efforts, on several continents and over more than three decades, to resolve international conflicts</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Masatoshi</t>
@@ -2561,10 +2562,10 @@
     <t>https://en.wikipedia.org/wiki/Masatoshi_Koshiba</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for pioneering contributions to astrophysics, in particular for the detection of cosmic neutrinos
 AWARD YEAR: 2002
-MOTIVATION: for pioneering contributions to astrophysics, in particular for the detection of cosmic neutrinos</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>May-Britt</t>
@@ -2651,10 +2652,10 @@
     <t>https://en.wikipedia.org/wiki/Mo_Yan</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: who with hallucinatory realism merges folk tales, history and the contemporary
 AWARD YEAR: 2012
-MOTIVATION: who with hallucinatory realism merges folk tales, history and the contemporary</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Mohamed</t>
@@ -2669,10 +2670,10 @@
     <t>https://en.wikipedia.org/wiki/Mohamed_ElBaradei</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for their efforts to prevent nuclear energy from being used for military purposes and to ensure that nuclear energy for peaceful purposes is used in the safest possible way
 AWARD YEAR: 2005
-MOTIVATION: for their efforts to prevent nuclear energy from being used for military purposes and to ensure that nuclear energy for peaceful purposes is used in the safest possible way</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Morten</t>
@@ -2708,10 +2709,10 @@
     <t>https://en.wikipedia.org/wiki/Muhammad_Yunus</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for their efforts to create economic and social development from below
 AWARD YEAR: 2006
-MOTIVATION: for their efforts to create economic and social development from below</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Nadia</t>
@@ -2738,10 +2739,10 @@
     <t>https://en.wikipedia.org/wiki/Narges_Mohammadi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for her fight against the oppression of women in Iran and her fight to promote human rights and freedom for all
 AWARD YEAR: 2023
-MOTIVATION: for her fight against the oppression of women in Iran and her fight to promote human rights and freedom for all</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Olga</t>
@@ -2756,10 +2757,10 @@
     <t>https://en.wikipedia.org/wiki/Olga_Tokarczuk</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for a narrative imagination that with encyclopedic passion represents the crossing of boundaries as a form of life
 AWARD YEAR: 2018
-MOTIVATION: for a narrative imagination that with encyclopedic passion represents the crossing of boundaries as a form of life</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Oliver E.</t>
@@ -2774,10 +2775,10 @@
     <t>https://en.wikipedia.org/wiki/Oliver_E._Williamson</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for his analysis of economic governance, especially the boundaries of the firm
 AWARD YEAR: 2009
-MOTIVATION: for his analysis of economic governance, especially the boundaries of the firm</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Oliver</t>
@@ -2813,10 +2814,10 @@
     <t>https://en.wikipedia.org/wiki/Orhan_Pamuk</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: who in the quest for the melancholic soul of his native city has discovered new symbols for the clash and interlacing of cultures
 AWARD YEAR: 2006
-MOTIVATION: who in the quest for the melancholic soul of his native city has discovered new symbols for the clash and interlacing of cultures</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Osamu</t>
@@ -2843,11 +2844,11 @@
     <t>https://en.wikipedia.org/wiki/Patrick_Modiano</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for the art of memory with which he has evoked the most ungraspable human destinies and_x000D_
+uncovered the life-world of the occupation
 AWARD YEAR: 2014
-MOTIVATION: for the art of memory with which he has evoked the most ungraspable human destinies and_x000D_
-uncovered the life-world of the occupation</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Paul C.</t>
@@ -2862,10 +2863,10 @@
     <t>https://en.wikipedia.org/wiki/Paul_Lauterbur</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries concerning magnetic resonance imaging
 AWARD YEAR: 2003
-MOTIVATION: for their discoveries concerning magnetic resonance imaging</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Paul</t>
@@ -2880,10 +2881,10 @@
     <t>https://en.wikipedia.org/wiki/Paul_Krugman</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for his analysis of trade patterns and location of economic activity
 AWARD YEAR: 2008
-MOTIVATION: for his analysis of trade patterns and location of economic activity</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Paul M.</t>
@@ -2898,10 +2899,10 @@
     <t>https://en.wikipedia.org/wiki/Paul_Romer</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for integrating technological innovations into long-run macroeconomic analysis
 AWARD YEAR: 2018
-MOTIVATION: for integrating technological innovations into long-run macroeconomic analysis</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Modrich</t>
@@ -2922,10 +2923,10 @@
     <t>https://en.wikipedia.org/wiki/Paul_Milgrom</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for improvements to auction theory and inventions of new auction formats
 AWARD YEAR: 2020
-MOTIVATION: for improvements to auction theory and inventions of new auction formats</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Peter A.</t>
@@ -2949,10 +2950,10 @@
     <t>https://en.wikipedia.org/wiki/Peter_Agre</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the discovery of water channels
 AWARD YEAR: 2003
-MOTIVATION: for the discovery of water channels</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Grünberg</t>
@@ -2973,10 +2974,10 @@
     <t>https://en.wikipedia.org/wiki/Peter_Handke</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for an influential work that with linguistic ingenuity has explored the periphery and the specificity of human experience
 AWARD YEAR: 2019
-MOTIVATION: for an influential work that with linguistic ingenuity has explored the periphery and the specificity of human experience</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Higgs</t>
@@ -3036,10 +3037,10 @@
     <t>https://en.wikipedia.org/wiki/Ralph_M._Steinman</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for his discovery of the dendritic cell and its role in adaptive immunity
 AWARD YEAR: 2011
-MOTIVATION: for his discovery of the dendritic cell and its role in adaptive immunity</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Randy W.</t>
@@ -3090,10 +3091,10 @@
     <t>https://en.wikipedia.org/wiki/Riccardo_Giacconi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for pioneering contributions to astrophysics, which have led to the discovery of cosmic X-ray sources
 AWARD YEAR: 2002
-MOTIVATION: for pioneering contributions to astrophysics, which have led to the discovery of cosmic X-ray sources</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Richard</t>
@@ -3132,10 +3133,10 @@
     <t>https://en.wikipedia.org/wiki/Richard_Thaler</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for his contributions to behavioural economics
 AWARD YEAR: 2017
-MOTIVATION: for his contributions to behavioural economics</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Henderson</t>
@@ -3159,10 +3160,10 @@
     <t>https://en.wikipedia.org/wiki/Richard_R._Schrock</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for the development of the metathesis method in organic synthesis
 AWARD YEAR: 2005
-MOTIVATION: for the development of the metathesis method in organic synthesis</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Robert</t>
@@ -3189,10 +3190,10 @@
     <t>https://en.wikipedia.org/wiki/Robert_F._Engle</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for methods of analyzing economic time series with time-varying volatility (ARCH)
 AWARD YEAR: 2003
-MOTIVATION: for methods of analyzing economic time series with time-varying volatility (ARCH)</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Robert G.</t>
@@ -3207,10 +3208,10 @@
     <t>https://en.wikipedia.org/wiki/Robert_G._Edwards</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for the development of in vitro fertilization
 AWARD YEAR: 2010
-MOTIVATION: for the development of in vitro fertilization</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Robert H.</t>
@@ -3237,10 +3238,10 @@
     <t>https://en.wikipedia.org/wiki/Robert_Aumann</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for having enhanced our understanding of conflict and cooperation through game-theory analysis
 AWARD YEAR: 2005
-MOTIVATION: for having enhanced our understanding of conflict and cooperation through game-theory analysis</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Lefkowitz</t>
@@ -3273,10 +3274,10 @@
     <t>https://en.wikipedia.org/wiki/Roderick_MacKinnon</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for structural and mechanistic studies of ion channels
 AWARD YEAR: 2003
-MOTIVATION: for structural and mechanistic studies of ion channels</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Roger B.</t>
@@ -3303,10 +3304,10 @@
     <t>https://en.wikipedia.org/wiki/Roger_D._Kornberg</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Chemistry
+    <t>CATEGORY: Chemistry
+MOTIVATION: for his studies of the molecular basis of eukaryotic transcription
 AWARD YEAR: 2006
-MOTIVATION: for his studies of the molecular basis of eukaryotic transcription</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Roger</t>
@@ -3321,10 +3322,10 @@
     <t>https://en.wikipedia.org/wiki/Roger_Penrose</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery that black hole formation is a robust prediction of the general theory of relativity
 AWARD YEAR: 2020
-MOTIVATION: for the discovery that black hole formation is a robust prediction of the general theory of relativity</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Roger Y.</t>
@@ -3351,10 +3352,10 @@
     <t>https://en.wikipedia.org/wiki/Roy_J._Glauber</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for his contribution to the quantum theory of optical coherence
 AWARD YEAR: 2005
-MOTIVATION: for his contribution to the quantum theory of optical coherence</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Satoshi</t>
@@ -3369,10 +3370,10 @@
     <t>https://en.wikipedia.org/wiki/Satoshi_Ōmura</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for their discoveries concerning a novel therapy against infections caused by roundworm parasites
 AWARD YEAR: 2015
-MOTIVATION: for their discoveries concerning a novel therapy against infections caused by roundworm parasites</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Saul</t>
@@ -3411,10 +3412,10 @@
     <t>https://en.wikipedia.org/wiki/Shinya_Yamanaka</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for the discovery that mature cells can be reprogrammed to become pluripotent
 AWARD YEAR: 2012
-MOTIVATION: for the discovery that mature cells can be reprogrammed to become pluripotent</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Shirin</t>
@@ -3429,10 +3430,10 @@
     <t>https://en.wikipedia.org/wiki/Shirin_Ebadi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for her efforts for democracy and human rights. She has focused especially on the struggle for the rights of women and children
 AWARD YEAR: 2003
-MOTIVATION: for her efforts for democracy and human rights. She has focused especially on the struggle for the rights of women and children</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Shuji</t>
@@ -3540,10 +3541,10 @@
     <t>https://en.wikipedia.org/wiki/Svante_Pääbo</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for his discoveries concerning the genomes of extinct hominins and human evolution
 AWARD YEAR: 2022
-MOTIVATION: for his discoveries concerning the genomes of extinct hominins and human evolution</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Svetlana</t>
@@ -3558,10 +3559,10 @@
     <t>https://en.wikipedia.org/wiki/Svetlana_Alexievich</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: for her polyphonic writings, a monument to suffering and courage in our time
 AWARD YEAR: 2015
-MOTIVATION: for her polyphonic writings, a monument to suffering and courage in our time</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Sydney</t>
@@ -3702,10 +3703,10 @@
     <t>https://en.wikipedia.org/wiki/Tomas_Tranströmer</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Literature
+    <t>CATEGORY: Literature
+MOTIVATION: because, through his condensed, translucent images, he gives us fresh access to reality
 AWARD YEAR: 2011
-MOTIVATION: because, through his condensed, translucent images, he gives us fresh access to reality</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Toshihide</t>
@@ -3732,10 +3733,10 @@
     <t>https://en.wikipedia.org/wiki/Tu_Youyou</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for her discoveries concerning a novel therapy against Malaria
 AWARD YEAR: 2015
-MOTIVATION: for her discoveries concerning a novel therapy against Malaria</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Venkatraman</t>
@@ -3759,10 +3760,10 @@
     <t>https://en.wikipedia.org/wiki/Vernon_L._Smith</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for having established laboratory experiments as a tool in empirical economic analysis, especially in the study of alternative market mechanisms
 AWARD YEAR: 2002
-MOTIVATION: for having established laboratory experiments as a tool in empirical economic analysis, especially in the study of alternative market mechanisms</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Vitaly L.</t>
@@ -3789,10 +3790,10 @@
     <t>https://en.wikipedia.org/wiki/Wangari_Maathai</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Peace
+    <t>CATEGORY: Peace
+MOTIVATION: for her contribution to sustainable development, democracy and peace
 AWARD YEAR: 2004
-MOTIVATION: for her contribution to sustainable development, democracy and peace</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Willard S.</t>
@@ -3831,10 +3832,10 @@
     <t>https://en.wikipedia.org/wiki/William_Nordhaus</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Economic Sciences
+    <t>CATEGORY: Economic Sciences
+MOTIVATION: for integrating climate change into long-run macroeconomic analysis
 AWARD YEAR: 2018
-MOTIVATION: for integrating climate change into long-run macroeconomic analysis</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>William E.</t>
@@ -3873,10 +3874,10 @@
     <t>https://en.wikipedia.org/wiki/Yoichiro_Nambu</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physics
+    <t>CATEGORY: Physics
+MOTIVATION: for the discovery of the mechanism of spontaneous broken symmetry in subatomic physics
 AWARD YEAR: 2008
-MOTIVATION: for the discovery of the mechanism of spontaneous broken symmetry in subatomic physics</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Yoshinori</t>
@@ -3891,10 +3892,10 @@
     <t>https://en.wikipedia.org/wiki/Yoshinori_Ohsumi</t>
   </si>
   <si>
-    <t>PRIZE STATUS: received
-CATEGORY: Physiology or Medicine
+    <t>CATEGORY: Physiology or Medicine
+MOTIVATION: for his discoveries of mechanisms for autophagy
 AWARD YEAR: 2016
-MOTIVATION: for his discoveries of mechanisms for autophagy</t>
+PRIZE STATUS: received</t>
   </si>
   <si>
     <t>Yves</t>
@@ -3904,6 +3905,93 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Yves_Chauvin</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Economic Sciences</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>Peace</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Physiology or Medicine</t>
   </si>
 </sst>
 </file>
@@ -3992,6 +4080,519 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Gender distribution of Nobel Prize winners</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Charts Data'!$A$1:$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>female</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>male</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Charts Data'!$B$1:$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>221</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Nobel Prizes won in given years</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Charts Data'!$D$1:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Charts Data'!$E$1:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Nobel Prizes won for a given categories</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Charts Data'!$G$1:$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Chemistry</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Economic Sciences</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Literature</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Peace</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Physics</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Physiology or Medicine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Charts Data'!$H$1:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9693,5 +10294,251 @@
     <hyperlink ref="E257" r:id="rId256"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId257"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="H1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>221</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1172</v>
+      </c>
+      <c r="H2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="D3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="D4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1174</v>
+      </c>
+      <c r="H4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="D5" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="D6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1176</v>
+      </c>
+      <c r="H6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="D7" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="D8" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="D9" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="D10" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="D11" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="D12" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="D13" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="D14" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="D15" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="D16" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="D19" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5">
+      <c r="D21" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5">
+      <c r="D22" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5">
+      <c r="D23" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>